<commit_message>
Fixing issues the smoke test failed due to test data
</commit_message>
<xml_diff>
--- a/testData/Hana_T69.xlsx
+++ b/testData/Hana_T69.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27830"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A45C84D2-8094-4714-8283-84FE3CD661A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A732B291-1B7D-4442-9EB7-22A211E47D5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -56,7 +56,7 @@
     <t>12345~Yellow Roses Standard~10.00~169513~true~false~Item~1801201</t>
   </si>
   <si>
-    <t>RSS-Rose Flowers -82</t>
+    <t>RSS-Rose Flowers -80</t>
   </si>
 </sst>
 </file>
@@ -435,7 +435,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Implement clear method in all the textbox field and implement base64 on extent report
</commit_message>
<xml_diff>
--- a/testData/Hana_T69.xlsx
+++ b/testData/Hana_T69.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27830"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A732B291-1B7D-4442-9EB7-22A211E47D5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5CC26FA-0614-4549-A1C3-5818438CCB4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4800" yWindow="1510" windowWidth="14400" windowHeight="7270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -47,16 +47,16 @@
     <t>Stuart Ben</t>
   </si>
   <si>
-    <t>RSS</t>
-  </si>
-  <si>
     <t>prodtile</t>
   </si>
   <si>
-    <t>12345~Yellow Roses Standard~10.00~169513~true~false~Item~1801201</t>
-  </si>
-  <si>
-    <t>RSS-Rose Flowers -80</t>
+    <t>TAI</t>
+  </si>
+  <si>
+    <t>Test Automation Item Deluxe</t>
+  </si>
+  <si>
+    <t>35486~Violet&amp;Roses Standard~21.00~169514~true~false~Item~1801202</t>
   </si>
 </sst>
 </file>
@@ -434,8 +434,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -444,7 +444,7 @@
     <col min="2" max="2" width="19.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.453125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="61.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -465,7 +465,7 @@
         <v>6</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>0</v>
@@ -482,13 +482,13 @@
         <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>1</v>

</xml_diff>